<commit_message>
cleaning up and refactoring for release
</commit_message>
<xml_diff>
--- a/data/ideophones_guessability.xlsx
+++ b/data/ideophones_guessability.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stell\Dropbox\triangulating_iconicity\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Data\R\triangulating_iconicity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AC7485-FC1E-421A-A905-8D8FB0E349B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392"/>
   </bookViews>
   <sheets>
     <sheet name="ideophones_meta" sheetId="1" r:id="rId1"/>
@@ -26,8 +25,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="language-top-ideophones" type="6" refreshedVersion="4" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="language-top-ideophones" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="1257" sourceFile="D:\Dropbox\Data\R\Ideophones_meta\out\language-top-ideophones.txt" comma="1">
       <textFields count="6">
         <textField/>
@@ -810,7 +809,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -844,7 +843,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -860,11 +859,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="language-top-ideophones" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="language-top-ideophones" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -939,23 +938,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -991,23 +973,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1183,27 +1148,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E242"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B114" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A217" sqref="A217"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.68359375" customWidth="1"/>
-    <col min="2" max="2" width="5.578125" customWidth="1"/>
-    <col min="3" max="3" width="8.41796875" customWidth="1"/>
-    <col min="4" max="4" width="10.26171875" customWidth="1"/>
-    <col min="5" max="5" width="8.83984375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>195</v>
       </c>
@@ -1220,7 +1184,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>214</v>
       </c>
@@ -1237,7 +1201,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1254,7 +1218,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1271,7 +1235,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1288,7 +1252,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1305,7 +1269,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>206</v>
       </c>
@@ -1322,7 +1286,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>209</v>
       </c>
@@ -1339,7 +1303,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>225</v>
       </c>
@@ -1356,7 +1320,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1373,7 +1337,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1390,7 +1354,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1407,7 +1371,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1424,7 +1388,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>221</v>
       </c>
@@ -1441,7 +1405,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>220</v>
       </c>
@@ -1458,7 +1422,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>212</v>
       </c>
@@ -1472,7 +1436,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>199</v>
       </c>
@@ -1489,7 +1453,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>206</v>
       </c>
@@ -1506,7 +1470,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1523,7 +1487,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1540,7 +1504,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>99</v>
       </c>
@@ -1557,7 +1521,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1574,7 +1538,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1591,7 +1555,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>196</v>
       </c>
@@ -1608,7 +1572,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>205</v>
       </c>
@@ -1622,7 +1586,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>203</v>
       </c>
@@ -1639,7 +1603,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>207</v>
       </c>
@@ -1656,7 +1620,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1673,7 +1637,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1690,7 +1654,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>192</v>
       </c>
@@ -1707,7 +1671,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -1724,7 +1688,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>167</v>
       </c>
@@ -1741,7 +1705,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1758,7 +1722,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1775,7 +1739,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -1792,7 +1756,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>249</v>
       </c>
@@ -1809,7 +1773,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1826,7 +1790,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -1843,7 +1807,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>229</v>
       </c>
@@ -1860,7 +1824,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>222</v>
       </c>
@@ -1877,7 +1841,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>200</v>
       </c>
@@ -1894,7 +1858,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>232</v>
       </c>
@@ -1911,7 +1875,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>197</v>
       </c>
@@ -1928,7 +1892,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>202</v>
       </c>
@@ -1945,7 +1909,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>227</v>
       </c>
@@ -1962,7 +1926,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>213</v>
       </c>
@@ -1979,7 +1943,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>22</v>
       </c>
@@ -1996,7 +1960,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -2013,7 +1977,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>221</v>
       </c>
@@ -2030,7 +1994,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>20</v>
       </c>
@@ -2047,7 +2011,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2064,7 +2028,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2081,7 +2045,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>23</v>
       </c>
@@ -2098,7 +2062,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>241</v>
       </c>
@@ -2115,7 +2079,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>46</v>
       </c>
@@ -2132,7 +2096,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>47</v>
       </c>
@@ -2149,7 +2113,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>44</v>
       </c>
@@ -2166,7 +2130,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>48</v>
       </c>
@@ -2183,7 +2147,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>28</v>
       </c>
@@ -2200,7 +2164,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>21</v>
       </c>
@@ -2217,7 +2181,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>45</v>
       </c>
@@ -2234,7 +2198,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>33</v>
       </c>
@@ -2251,7 +2215,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>170</v>
       </c>
@@ -2268,7 +2232,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>50</v>
       </c>
@@ -2285,7 +2249,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>198</v>
       </c>
@@ -2299,7 +2263,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>216</v>
       </c>
@@ -2313,7 +2277,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>218</v>
       </c>
@@ -2327,7 +2291,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>219</v>
       </c>
@@ -2341,7 +2305,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>153</v>
       </c>
@@ -2358,7 +2322,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>34</v>
       </c>
@@ -2375,7 +2339,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>36</v>
       </c>
@@ -2392,7 +2356,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>252</v>
       </c>
@@ -2409,7 +2373,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>35</v>
       </c>
@@ -2426,7 +2390,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>37</v>
       </c>
@@ -2443,7 +2407,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>190</v>
       </c>
@@ -2460,7 +2424,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>251</v>
       </c>
@@ -2477,7 +2441,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>140</v>
       </c>
@@ -2494,7 +2458,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>143</v>
       </c>
@@ -2511,7 +2475,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>148</v>
       </c>
@@ -2528,7 +2492,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>171</v>
       </c>
@@ -2545,7 +2509,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>179</v>
       </c>
@@ -2562,7 +2526,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>186</v>
       </c>
@@ -2579,7 +2543,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>102</v>
       </c>
@@ -2596,7 +2560,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>107</v>
       </c>
@@ -2613,7 +2577,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>112</v>
       </c>
@@ -2630,7 +2594,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>158</v>
       </c>
@@ -2647,7 +2611,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>164</v>
       </c>
@@ -2664,7 +2628,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>245</v>
       </c>
@@ -2681,7 +2645,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>201</v>
       </c>
@@ -2695,7 +2659,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>217</v>
       </c>
@@ -2709,7 +2673,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>204</v>
       </c>
@@ -2723,7 +2687,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>226</v>
       </c>
@@ -2737,7 +2701,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>117</v>
       </c>
@@ -2754,7 +2718,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>118</v>
       </c>
@@ -2771,7 +2735,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>125</v>
       </c>
@@ -2788,7 +2752,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>112</v>
       </c>
@@ -2805,7 +2769,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>131</v>
       </c>
@@ -2822,7 +2786,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>132</v>
       </c>
@@ -2839,7 +2803,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>135</v>
       </c>
@@ -2856,7 +2820,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>139</v>
       </c>
@@ -2873,7 +2837,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>144</v>
       </c>
@@ -2890,7 +2854,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>145</v>
       </c>
@@ -2907,7 +2871,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>152</v>
       </c>
@@ -2924,7 +2888,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>174</v>
       </c>
@@ -2941,7 +2905,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>175</v>
       </c>
@@ -2958,7 +2922,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>181</v>
       </c>
@@ -2975,7 +2939,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>101</v>
       </c>
@@ -2992,7 +2956,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>109</v>
       </c>
@@ -3009,7 +2973,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>232</v>
       </c>
@@ -3026,7 +2990,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>228</v>
       </c>
@@ -3040,7 +3004,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>230</v>
       </c>
@@ -3054,7 +3018,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>236</v>
       </c>
@@ -3071,7 +3035,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>157</v>
       </c>
@@ -3088,7 +3052,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>166</v>
       </c>
@@ -3105,7 +3069,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>115</v>
       </c>
@@ -3122,7 +3086,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>116</v>
       </c>
@@ -3139,7 +3103,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>250</v>
       </c>
@@ -3156,7 +3120,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>128</v>
       </c>
@@ -3173,7 +3137,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>130</v>
       </c>
@@ -3190,7 +3154,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>134</v>
       </c>
@@ -3207,7 +3171,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>136</v>
       </c>
@@ -3224,7 +3188,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>150</v>
       </c>
@@ -3241,7 +3205,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>168</v>
       </c>
@@ -3258,7 +3222,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>169</v>
       </c>
@@ -3275,7 +3239,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>172</v>
       </c>
@@ -3292,7 +3256,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>176</v>
       </c>
@@ -3309,7 +3273,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>182</v>
       </c>
@@ -3326,7 +3290,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>189</v>
       </c>
@@ -3343,7 +3307,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>98</v>
       </c>
@@ -3360,7 +3324,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>110</v>
       </c>
@@ -3377,7 +3341,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>113</v>
       </c>
@@ -3394,7 +3358,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>159</v>
       </c>
@@ -3411,7 +3375,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>161</v>
       </c>
@@ -3428,7 +3392,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>208</v>
       </c>
@@ -3442,7 +3406,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>231</v>
       </c>
@@ -3456,7 +3420,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>211</v>
       </c>
@@ -3470,7 +3434,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>223</v>
       </c>
@@ -3484,7 +3448,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>237</v>
       </c>
@@ -3501,7 +3465,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>185</v>
       </c>
@@ -3518,7 +3482,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>151</v>
       </c>
@@ -3535,7 +3499,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>146</v>
       </c>
@@ -3552,7 +3516,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>147</v>
       </c>
@@ -3569,7 +3533,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>187</v>
       </c>
@@ -3586,7 +3550,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>173</v>
       </c>
@@ -3603,7 +3567,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>100</v>
       </c>
@@ -3620,7 +3584,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>129</v>
       </c>
@@ -3637,7 +3601,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>178</v>
       </c>
@@ -3654,7 +3618,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>177</v>
       </c>
@@ -3671,7 +3635,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>180</v>
       </c>
@@ -3688,7 +3652,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>111</v>
       </c>
@@ -3705,7 +3669,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>105</v>
       </c>
@@ -3722,7 +3686,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>246</v>
       </c>
@@ -3739,7 +3703,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>244</v>
       </c>
@@ -3756,7 +3720,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>120</v>
       </c>
@@ -3773,7 +3737,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>119</v>
       </c>
@@ -3790,7 +3754,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>247</v>
       </c>
@@ -3807,7 +3771,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>141</v>
       </c>
@@ -3824,7 +3788,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>104</v>
       </c>
@@ -3841,7 +3805,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>163</v>
       </c>
@@ -3858,7 +3822,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>233</v>
       </c>
@@ -3875,7 +3839,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>133</v>
       </c>
@@ -3892,7 +3856,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="162" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>138</v>
       </c>
@@ -3909,7 +3873,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>149</v>
       </c>
@@ -3926,7 +3890,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>155</v>
       </c>
@@ -3943,7 +3907,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>160</v>
       </c>
@@ -3960,7 +3924,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>238</v>
       </c>
@@ -3977,7 +3941,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>184</v>
       </c>
@@ -3994,7 +3958,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>183</v>
       </c>
@@ -4011,7 +3975,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>188</v>
       </c>
@@ -4028,7 +3992,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>165</v>
       </c>
@@ -4045,7 +4009,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>127</v>
       </c>
@@ -4062,7 +4026,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>59</v>
       </c>
@@ -4079,7 +4043,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>103</v>
       </c>
@@ -4096,7 +4060,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>240</v>
       </c>
@@ -4113,7 +4077,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>156</v>
       </c>
@@ -4130,7 +4094,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>106</v>
       </c>
@@ -4147,7 +4111,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>123</v>
       </c>
@@ -4164,7 +4128,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>114</v>
       </c>
@@ -4181,7 +4145,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>137</v>
       </c>
@@ -4198,7 +4162,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>239</v>
       </c>
@@ -4215,7 +4179,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="181" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>108</v>
       </c>
@@ -4232,7 +4196,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>210</v>
       </c>
@@ -4249,7 +4213,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="183" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>57</v>
       </c>
@@ -4266,7 +4230,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="184" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>55</v>
       </c>
@@ -4283,7 +4247,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="185" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>53</v>
       </c>
@@ -4300,7 +4264,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>154</v>
       </c>
@@ -4317,7 +4281,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="187" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>121</v>
       </c>
@@ -4334,7 +4298,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="188" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>191</v>
       </c>
@@ -4351,7 +4315,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="189" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>122</v>
       </c>
@@ -4368,7 +4332,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="190" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>78</v>
       </c>
@@ -4385,7 +4349,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="191" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>52</v>
       </c>
@@ -4402,7 +4366,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>162</v>
       </c>
@@ -4419,7 +4383,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="193" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>56</v>
       </c>
@@ -4436,7 +4400,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>58</v>
       </c>
@@ -4453,7 +4417,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="195" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>76</v>
       </c>
@@ -4470,7 +4434,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>91</v>
       </c>
@@ -4487,7 +4451,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="197" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>90</v>
       </c>
@@ -4504,7 +4468,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>54</v>
       </c>
@@ -4521,7 +4485,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="199" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>124</v>
       </c>
@@ -4538,7 +4502,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="200" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>126</v>
       </c>
@@ -4555,7 +4519,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>89</v>
       </c>
@@ -4572,7 +4536,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>224</v>
       </c>
@@ -4589,7 +4553,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>215</v>
       </c>
@@ -4603,7 +4567,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>242</v>
       </c>
@@ -4620,7 +4584,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>243</v>
       </c>
@@ -4637,7 +4601,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="206" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>67</v>
       </c>
@@ -4654,7 +4618,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="207" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>68</v>
       </c>
@@ -4671,7 +4635,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>73</v>
       </c>
@@ -4688,7 +4652,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>253</v>
       </c>
@@ -4705,7 +4669,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="210" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>142</v>
       </c>
@@ -4722,7 +4686,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="211" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>60</v>
       </c>
@@ -4739,7 +4703,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>61</v>
       </c>
@@ -4756,7 +4720,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="213" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>62</v>
       </c>
@@ -4773,7 +4737,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>248</v>
       </c>
@@ -4790,7 +4754,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>92</v>
       </c>
@@ -4807,7 +4771,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="216" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>93</v>
       </c>
@@ -4824,7 +4788,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>74</v>
       </c>
@@ -4841,7 +4805,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>69</v>
       </c>
@@ -4858,7 +4822,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="219" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>70</v>
       </c>
@@ -4875,7 +4839,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="220" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>82</v>
       </c>
@@ -4892,7 +4856,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="221" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>77</v>
       </c>
@@ -4909,7 +4873,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>79</v>
       </c>
@@ -4926,7 +4890,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>80</v>
       </c>
@@ -4943,7 +4907,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="224" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>81</v>
       </c>
@@ -4960,7 +4924,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>94</v>
       </c>
@@ -4977,7 +4941,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>235</v>
       </c>
@@ -4994,7 +4958,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>71</v>
       </c>
@@ -5011,7 +4975,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>72</v>
       </c>
@@ -5028,7 +4992,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>63</v>
       </c>
@@ -5045,7 +5009,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>64</v>
       </c>
@@ -5062,7 +5026,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>83</v>
       </c>
@@ -5079,7 +5043,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="232" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>84</v>
       </c>
@@ -5096,7 +5060,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="233" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>95</v>
       </c>
@@ -5113,7 +5077,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>85</v>
       </c>
@@ -5130,7 +5094,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>86</v>
       </c>
@@ -5147,7 +5111,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>65</v>
       </c>
@@ -5164,7 +5128,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="237" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>96</v>
       </c>
@@ -5181,7 +5145,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>75</v>
       </c>
@@ -5198,7 +5162,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="239" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>66</v>
       </c>
@@ -5215,7 +5179,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="240" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>87</v>
       </c>
@@ -5232,7 +5196,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="241" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>88</v>
       </c>
@@ -5249,7 +5213,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="242" spans="1:5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>97</v>
       </c>
@@ -5267,14 +5231,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E242" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Japanese"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A205:J242">
+  <autoFilter ref="A1:E242"/>
+  <sortState ref="A205:J242">
     <sortCondition ref="A205"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5283,16 +5241,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C39" sqref="C2:C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>195</v>
       </c>
@@ -5300,7 +5258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5311,7 +5269,7 @@
         <v>0.82758620689655205</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5322,7 +5280,7 @@
         <v>0.75862068965517204</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5333,7 +5291,7 @@
         <v>0.72413793103448298</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5344,7 +5302,7 @@
         <v>0.86206896551724099</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5355,7 +5313,7 @@
         <v>0.79310344827586199</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5366,7 +5324,7 @@
         <v>0.68965517241379304</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5377,7 +5335,7 @@
         <v>0.75862068965517204</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5388,7 +5346,7 @@
         <v>0.82758620689655205</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5399,7 +5357,7 @@
         <v>0.65517241379310298</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5410,7 +5368,7 @@
         <v>0.82758620689655205</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5421,7 +5379,7 @@
         <v>0.931034482758621</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5432,7 +5390,7 @@
         <v>0.82758620689655205</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5443,7 +5401,7 @@
         <v>0.58620689655172398</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5454,7 +5412,7 @@
         <v>0.931034482758621</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5465,7 +5423,7 @@
         <v>0.48275862068965503</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5476,7 +5434,7 @@
         <v>0.55172413793103403</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5487,7 +5445,7 @@
         <v>0.86206896551724099</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5498,7 +5456,7 @@
         <v>0.75862068965517204</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5509,7 +5467,7 @@
         <v>0.96551724137931005</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5520,7 +5478,7 @@
         <v>0.41379310344827602</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5531,7 +5489,7 @@
         <v>0.72413793103448298</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5542,7 +5500,7 @@
         <v>0.68965517241379304</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5553,7 +5511,7 @@
         <v>0.72413793103448298</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5564,7 +5522,7 @@
         <v>0.72413793103448298</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5575,7 +5533,7 @@
         <v>0.86206896551724099</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5586,7 +5544,7 @@
         <v>0.89655172413793105</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5597,7 +5555,7 @@
         <v>0.79310344827586199</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5608,7 +5566,7 @@
         <v>0.55172413793103403</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5619,7 +5577,7 @@
         <v>0.44827586206896602</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5630,7 +5588,7 @@
         <v>0.931034482758621</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5641,7 +5599,7 @@
         <v>0.65517241379310298</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5652,7 +5610,7 @@
         <v>0.75862068965517204</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5663,7 +5621,7 @@
         <v>0.62068965517241403</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5674,7 +5632,7 @@
         <v>0.79310344827586199</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5685,7 +5643,7 @@
         <v>0.62068965517241403</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5696,7 +5654,7 @@
         <v>0.58620689655172398</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5707,7 +5665,7 @@
         <v>0.79310344827586199</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5724,12 +5682,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>